<commit_message>
se agregro las funcionalidades salir reiniciar y falta lo de las ayudas
</commit_message>
<xml_diff>
--- a/src/files/preguntas.xlsx
+++ b/src/files/preguntas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
   <si>
     <t>pregunta1</t>
   </si>
@@ -262,13 +262,25 @@
   </si>
   <si>
     <t>RESPUESTA</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +411,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -745,8 +765,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,8 +1133,8 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,8 +1153,8 @@
       <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>2</v>
+      <c r="F3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,8 +1173,8 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>3</v>
+      <c r="F4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,8 +1193,8 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>4</v>
+      <c r="F5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1192,8 +1213,8 @@
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="F6">
-        <v>1</v>
+      <c r="F6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,8 +1233,8 @@
       <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="F7">
-        <v>2</v>
+      <c r="F7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1232,8 +1253,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="F8">
-        <v>3</v>
+      <c r="F8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1252,8 +1273,8 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="F9">
-        <v>4</v>
+      <c r="F9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1272,8 +1293,8 @@
       <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F10">
-        <v>1</v>
+      <c r="F10" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1292,8 +1313,8 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>2</v>
+      <c r="F11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1312,8 +1333,8 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="F12">
-        <v>3</v>
+      <c r="F12" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,8 +1353,8 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13">
-        <v>4</v>
+      <c r="F13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,8 +1373,8 @@
       <c r="E14" t="s">
         <v>12</v>
       </c>
-      <c r="F14">
-        <v>1</v>
+      <c r="F14" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1372,8 +1393,8 @@
       <c r="E15" t="s">
         <v>13</v>
       </c>
-      <c r="F15">
-        <v>2</v>
+      <c r="F15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,9 +1413,12 @@
       <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
+      <c r="F16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se finalizo gran parte solo falta hacer pruebas y ver que ajusten emplear
</commit_message>
<xml_diff>
--- a/src/files/preguntas.xlsx
+++ b/src/files/preguntas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
   <si>
     <t>pregunta1</t>
   </si>
@@ -274,6 +274,54 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>PISTA</t>
+  </si>
+  <si>
+    <t>pista1</t>
+  </si>
+  <si>
+    <t>pista2</t>
+  </si>
+  <si>
+    <t>pista3</t>
+  </si>
+  <si>
+    <t>pista4</t>
+  </si>
+  <si>
+    <t>pista5</t>
+  </si>
+  <si>
+    <t>pista6</t>
+  </si>
+  <si>
+    <t>pista7</t>
+  </si>
+  <si>
+    <t>pista8</t>
+  </si>
+  <si>
+    <t>pista9</t>
+  </si>
+  <si>
+    <t>pista10</t>
+  </si>
+  <si>
+    <t>pista11</t>
+  </si>
+  <si>
+    <t>pista12</t>
+  </si>
+  <si>
+    <t>pista13</t>
+  </si>
+  <si>
+    <t>pista14</t>
+  </si>
+  <si>
+    <t>pista15</t>
   </si>
 </sst>
 </file>
@@ -1089,15 +1137,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1116,8 +1164,11 @@
       <c r="F1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1136,8 +1187,11 @@
       <c r="F2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1156,8 +1210,11 @@
       <c r="F3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1176,8 +1233,11 @@
       <c r="F4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1196,8 +1256,11 @@
       <c r="F5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1216,8 +1279,11 @@
       <c r="F6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1236,8 +1302,11 @@
       <c r="F7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1256,8 +1325,11 @@
       <c r="F8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1276,8 +1348,11 @@
       <c r="F9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1296,8 +1371,11 @@
       <c r="F10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1316,8 +1394,11 @@
       <c r="F11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1336,8 +1417,11 @@
       <c r="F12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1356,8 +1440,11 @@
       <c r="F13" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1376,8 +1463,11 @@
       <c r="F14" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1396,8 +1486,11 @@
       <c r="F15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1415,6 +1508,9 @@
       </c>
       <c r="F16" t="s">
         <v>83</v>
+      </c>
+      <c r="G16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se agregro sonido y alertas primera prueba para sacar a produccion
</commit_message>
<xml_diff>
--- a/src/files/preguntas.xlsx
+++ b/src/files/preguntas.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
   <si>
-    <t>pregunta1</t>
-  </si>
-  <si>
     <t>pregunta2</t>
   </si>
   <si>
@@ -66,24 +63,12 @@
     <t>pregunta15</t>
   </si>
   <si>
-    <t>resa1</t>
-  </si>
-  <si>
     <t>resb2</t>
   </si>
   <si>
     <t>resc3</t>
   </si>
   <si>
-    <t>resb1</t>
-  </si>
-  <si>
-    <t>resc1</t>
-  </si>
-  <si>
-    <t>resd1</t>
-  </si>
-  <si>
     <t>resa2</t>
   </si>
   <si>
@@ -279,9 +264,6 @@
     <t>PISTA</t>
   </si>
   <si>
-    <t>pista1</t>
-  </si>
-  <si>
     <t>pista2</t>
   </si>
   <si>
@@ -322,6 +304,24 @@
   </si>
   <si>
     <t>pista15</t>
+  </si>
+  <si>
+    <t>primer color del bandera de colombia</t>
+  </si>
+  <si>
+    <t>rojo</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>amarillo</t>
+  </si>
+  <si>
+    <t>el color del oro</t>
   </si>
 </sst>
 </file>
@@ -1140,377 +1140,381 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>80</v>
-      </c>
-      <c r="G1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>